<commit_message>
creating more tables and reworking connection
</commit_message>
<xml_diff>
--- a/database/list.xlsx
+++ b/database/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Flutter Projects\cosmetics_shop\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E826F3-11D0-453E-99B3-A33FCD9C77F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D5492B-E4A2-4D91-8D37-0981646D9B5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{0F8F40B5-1CDC-D64B-A38F-578BA2581425}"/>
   </bookViews>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926D11D8-0C43-6B40-B1F4-FEF970495C3F}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -819,10 +819,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCA52F1-DBFA-454C-8318-775680BBEB5C}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -887,10 +887,16 @@
         <v>50</v>
       </c>
     </row>
+    <row r="6" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ add records to cart&fav tables | bug fix
</commit_message>
<xml_diff>
--- a/database/list.xlsx
+++ b/database/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Flutter Projects\cosmetics_shop\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D5492B-E4A2-4D91-8D37-0981646D9B5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BE3B96-2408-4374-9E58-EE129FC9A1D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{0F8F40B5-1CDC-D64B-A38F-578BA2581425}"/>
   </bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -223,13 +220,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -283,29 +274,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{995FBAA1-B75A-BF4F-A30B-B2FBA62B2C28}" name="Products" displayName="Products" ref="A1:H7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:H7" xr:uid="{2AA5177D-93EB-6046-83B8-D2A21AC8B782}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{CA2C1C80-CEC0-1A48-957B-565D62670CF5}" name="id" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{996174B9-49E3-C44E-8BD7-5ABF84372721}" name="name" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{83ED3A9A-6F46-154A-95CC-6C2937654638}" name="categoryID" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{317F1B87-79F0-0A47-9756-11D994A16A41}" name="manufacter" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{20DE4804-C1CF-9F4D-B6ED-2DE1A5A9B461}" name="price" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{36298C89-1DA9-2544-9FC7-C0D9C6A00EC0}" name="imagePath" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{CD72B621-5B6B-AB44-BA86-A0A2232ED1D9}" name="shortDescription" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{3D6DDBA5-5D3E-974D-A94F-8178745CBE32}" name="longDescription" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{995FBAA1-B75A-BF4F-A30B-B2FBA62B2C28}" name="Products" displayName="Products" ref="A1:G7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:G7" xr:uid="{2AA5177D-93EB-6046-83B8-D2A21AC8B782}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{CA2C1C80-CEC0-1A48-957B-565D62670CF5}" name="name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{996174B9-49E3-C44E-8BD7-5ABF84372721}" name="categoryID" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{83ED3A9A-6F46-154A-95CC-6C2937654638}" name="manufacter" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{317F1B87-79F0-0A47-9756-11D994A16A41}" name="price" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{20DE4804-C1CF-9F4D-B6ED-2DE1A5A9B461}" name="imagePath" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{36298C89-1DA9-2544-9FC7-C0D9C6A00EC0}" name="shortDescription" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{CD72B621-5B6B-AB44-BA86-A0A2232ED1D9}" name="longDescription" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3F90FAD-97EE-4F53-B13F-480EA3338696}" name="Products2" displayName="Products2" ref="A1:C5" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C5" xr:uid="{EA01BB9C-CDCA-4B1C-A32F-CBB907130A71}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{99917D01-1BFF-460B-B61F-96DE825D477E}" name="id" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{F7DC2A0A-9A39-4A99-B8EA-C0C7B2E07015}" name="name" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{97F2CFAE-3B96-4CFC-A804-1E51708BFE3E}" name="imagePath" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3F90FAD-97EE-4F53-B13F-480EA3338696}" name="Products2" displayName="Products2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:B5" xr:uid="{EA01BB9C-CDCA-4B1C-A32F-CBB907130A71}"/>
+  <tableColumns count="2">
+    <tableColumn id="2" xr3:uid="{F7DC2A0A-9A39-4A99-B8EA-C0C7B2E07015}" name="name" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{97F2CFAE-3B96-4CFC-A804-1E51708BFE3E}" name="imagePath" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -608,33 +597,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926D11D8-0C43-6B40-B1F4-FEF970495C3F}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.796875" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="12.69921875" customWidth="1"/>
-    <col min="6" max="6" width="41.5" customWidth="1"/>
-    <col min="7" max="7" width="33.5" customWidth="1"/>
-    <col min="8" max="8" width="57" customWidth="1"/>
+    <col min="1" max="1" width="23.796875" customWidth="1"/>
+    <col min="2" max="2" width="25.796875" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="20.8984375" customWidth="1"/>
+    <col min="5" max="5" width="40.59765625" customWidth="1"/>
+    <col min="6" max="6" width="46.3984375" customWidth="1"/>
+    <col min="7" max="7" width="64.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -648,167 +636,146 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="78" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="78" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="4" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="78" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="5" spans="1:7" ht="91.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="91.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="94.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="94.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -819,78 +786,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCA52F1-DBFA-454C-8318-775680BBEB5C}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:2" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
wipe data on init function
</commit_message>
<xml_diff>
--- a/database/list.xlsx
+++ b/database/list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Flutter Projects\cosmetics_shop\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moryoka/Documents/Flutter Projects/cosmetics_shop/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BE3B96-2408-4374-9E58-EE129FC9A1D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B590AA8F-FF44-A94A-943B-00BFB000B146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{0F8F40B5-1CDC-D64B-A38F-578BA2581425}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{0F8F40B5-1CDC-D64B-A38F-578BA2581425}"/>
   </bookViews>
   <sheets>
     <sheet name="productsList" sheetId="1" r:id="rId1"/>
@@ -277,24 +277,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{995FBAA1-B75A-BF4F-A30B-B2FBA62B2C28}" name="Products" displayName="Products" ref="A1:G7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:G7" xr:uid="{2AA5177D-93EB-6046-83B8-D2A21AC8B782}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CA2C1C80-CEC0-1A48-957B-565D62670CF5}" name="name" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{996174B9-49E3-C44E-8BD7-5ABF84372721}" name="categoryID" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{83ED3A9A-6F46-154A-95CC-6C2937654638}" name="manufacter" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{317F1B87-79F0-0A47-9756-11D994A16A41}" name="price" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{20DE4804-C1CF-9F4D-B6ED-2DE1A5A9B461}" name="imagePath" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{36298C89-1DA9-2544-9FC7-C0D9C6A00EC0}" name="shortDescription" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{CD72B621-5B6B-AB44-BA86-A0A2232ED1D9}" name="longDescription" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CA2C1C80-CEC0-1A48-957B-565D62670CF5}" name="name" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{996174B9-49E3-C44E-8BD7-5ABF84372721}" name="categoryID" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{83ED3A9A-6F46-154A-95CC-6C2937654638}" name="manufacter" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{317F1B87-79F0-0A47-9756-11D994A16A41}" name="price" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{20DE4804-C1CF-9F4D-B6ED-2DE1A5A9B461}" name="imagePath" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{36298C89-1DA9-2544-9FC7-C0D9C6A00EC0}" name="shortDescription" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{CD72B621-5B6B-AB44-BA86-A0A2232ED1D9}" name="longDescription" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3F90FAD-97EE-4F53-B13F-480EA3338696}" name="Products2" displayName="Products2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3F90FAD-97EE-4F53-B13F-480EA3338696}" name="Products2" displayName="Products2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B5" xr:uid="{EA01BB9C-CDCA-4B1C-A32F-CBB907130A71}"/>
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{F7DC2A0A-9A39-4A99-B8EA-C0C7B2E07015}" name="name" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{97F2CFAE-3B96-4CFC-A804-1E51708BFE3E}" name="imagePath" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F7DC2A0A-9A39-4A99-B8EA-C0C7B2E07015}" name="name" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{97F2CFAE-3B96-4CFC-A804-1E51708BFE3E}" name="imagePath" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -597,24 +597,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926D11D8-0C43-6B40-B1F4-FEF970495C3F}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="113" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.796875" customWidth="1"/>
-    <col min="2" max="2" width="25.796875" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="20.8984375" customWidth="1"/>
-    <col min="5" max="5" width="40.59765625" customWidth="1"/>
-    <col min="6" max="6" width="46.3984375" customWidth="1"/>
-    <col min="7" max="7" width="64.8984375" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" customWidth="1"/>
+    <col min="7" max="7" width="64.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="22.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,7 +637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -660,7 +660,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -683,7 +683,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -706,7 +706,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="91.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="91" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -729,7 +729,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="94.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -752,7 +752,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -775,7 +775,6 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -792,13 +791,13 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,7 +805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="50.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
@@ -814,7 +813,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="51.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
@@ -822,7 +821,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -830,7 +829,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="56.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -838,7 +837,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>

</xml_diff>

<commit_message>
change the tables name
</commit_message>
<xml_diff>
--- a/database/list.xlsx
+++ b/database/list.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moryoka/Documents/Flutter Projects/cosmetics_shop/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B590AA8F-FF44-A94A-943B-00BFB000B146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE1825C-9EB5-104D-9EF2-EC29D119B7C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{0F8F40B5-1CDC-D64B-A38F-578BA2581425}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" activeTab="1" xr2:uid="{0F8F40B5-1CDC-D64B-A38F-578BA2581425}"/>
   </bookViews>
   <sheets>
-    <sheet name="productsList" sheetId="1" r:id="rId1"/>
-    <sheet name="categoriesList" sheetId="2" r:id="rId2"/>
+    <sheet name="products" sheetId="1" r:id="rId1"/>
+    <sheet name="categories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -599,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926D11D8-0C43-6B40-B1F4-FEF970495C3F}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="113" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="113" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -787,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCA52F1-DBFA-454C-8318-775680BBEB5C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>